<commit_message>
Refacto POM create account
</commit_message>
<xml_diff>
--- a/Ressources/SFCC/TestData/2_createAccount.xlsx
+++ b/Ressources/SFCC/TestData/2_createAccount.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onepoint365-my.sharepoint.com/personal/s_ramos-izquierdo_groupeonepoint_com/Documents/Bureau/Clarins/Outils/clarins_auto_uat_ihm/Jeux de donnees/SFCC/NewAccount/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onepoint365-my.sharepoint.com/personal/s_ramos-izquierdo_groupeonepoint_com/Documents/Bureau/Clarins/Outils/clarins_auto_uat_ihm/Ressources/SFCC/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="529" documentId="8_{F2498E7F-A211-5648-BD84-328060702354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71D70627-F1FE-4B0E-B400-8F8D2A0C1866}"/>
+  <xr:revisionPtr revIDLastSave="556" documentId="8_{F2498E7F-A211-5648-BD84-328060702354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB6042C0-5510-4CFA-B527-54C9DFB882EB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4DDB3DD0-E88E-8949-89B8-E2C45E0A4C00}"/>
   </bookViews>
@@ -36,26 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="40">
   <si>
     <t>*** Test Cases ***</t>
   </si>
   <si>
-    <t>${BirthDate}</t>
-  </si>
-  <si>
-    <t>${LastName}</t>
-  </si>
-  <si>
-    <t>${FirstName}</t>
-  </si>
-  <si>
-    <t>${mypassword}</t>
-  </si>
-  <si>
-    <t>${Email}</t>
-  </si>
-  <si>
     <t>auto</t>
   </si>
   <si>
@@ -86,9 +71,6 @@
     <t>CHE</t>
   </si>
   <si>
-    <t>${emailOption}</t>
-  </si>
-  <si>
     <t>${isLoyaltyMember}</t>
   </si>
   <si>
@@ -144,6 +126,36 @@
   </si>
   <si>
     <t xml:space="preserve">Incident car redirection sur URL FRA </t>
+  </si>
+  <si>
+    <t>UC9_SFCC_Create_Account_POL_UAT</t>
+  </si>
+  <si>
+    <t>${firstName}</t>
+  </si>
+  <si>
+    <t>${lastName}</t>
+  </si>
+  <si>
+    <t>${email}</t>
+  </si>
+  <si>
+    <t>${password}</t>
+  </si>
+  <si>
+    <t>${birthDate}</t>
+  </si>
+  <si>
+    <t>${emailOptin}</t>
+  </si>
+  <si>
+    <t>POL</t>
+  </si>
+  <si>
+    <t>${SMSOptin}</t>
+  </si>
+  <si>
+    <t>${phoneNumber}</t>
   </si>
 </sst>
 </file>
@@ -700,396 +712,463 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6BC4A3E-ED2A-A240-8C79-297922065A66}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="45" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.19921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.59765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="80.296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.796875" style="1"/>
+    <col min="8" max="8" width="22.19921875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.19921875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="27.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="80.296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="11" customFormat="1" ht="19.05" customHeight="1">
+    <row r="1" spans="1:15" s="11" customFormat="1" ht="19.05" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="21">
+      <c r="A2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="N2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="7"/>
+    </row>
+    <row r="3" spans="1:15" ht="21">
+      <c r="A3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="21">
+      <c r="A4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="7"/>
+    </row>
+    <row r="5" spans="1:15" ht="21">
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="7"/>
+    </row>
+    <row r="6" spans="1:15" ht="21">
+      <c r="A6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="8" t="s">
+      <c r="N6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="21">
+      <c r="A7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="13" t="s">
+      <c r="K7" s="5"/>
+      <c r="L7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="21">
+      <c r="A8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="21">
+      <c r="A9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O9" s="7"/>
+    </row>
+    <row r="10" spans="1:15" ht="21">
+      <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="13" t="s">
-        <v>32</v>
-      </c>
+      <c r="B10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" s="5"/>
+      <c r="M10" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="7"/>
     </row>
-    <row r="2" spans="1:13" ht="21">
-      <c r="A2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="7"/>
-    </row>
-    <row r="3" spans="1:13" ht="21">
-      <c r="A3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="21">
-      <c r="A4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="7"/>
-    </row>
-    <row r="5" spans="1:13" ht="21">
-      <c r="A5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="M5" s="7"/>
-    </row>
-    <row r="6" spans="1:13" ht="21">
-      <c r="A6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="21">
-      <c r="A7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="21">
-      <c r="A8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="21">
-      <c r="A9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="M9" s="7"/>
-    </row>
-    <row r="13" spans="1:13" ht="17.399999999999999">
-      <c r="M13" s="12"/>
+    <row r="13" spans="1:15" ht="17.399999999999999">
+      <c r="O13" s="12"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:J9">
+  <conditionalFormatting sqref="B2:L10">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
@@ -1097,24 +1176,24 @@
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" dxfId="3" priority="19" operator="equal">
+  <conditionalFormatting sqref="C1">
+    <cfRule type="cellIs" dxfId="3" priority="21" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="22" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2">
-    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
+  <conditionalFormatting sqref="M2">
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="M3" r:id="rId1" display="https://staging-clarins-ecommera.demandware.net/on/demandware.store/Sites-clarinsus-Site" xr:uid="{192CDE7C-4B7F-B146-A980-7F3F6489C6A4}"/>
+    <hyperlink ref="O3" r:id="rId1" display="https://staging-clarins-ecommera.demandware.net/on/demandware.store/Sites-clarinsus-Site" xr:uid="{192CDE7C-4B7F-B146-A980-7F3F6489C6A4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>